<commit_message>
new warm fall schedule
</commit_message>
<xml_diff>
--- a/notes/climate_chamber/schedule/warm_fall/WarmF25sept.xlsx
+++ b/notes/climate_chamber/schedule/warm_fall/WarmF25sept.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/Documents/github/fuelinex/notes/climate_chamber/schedule/warm_fall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476D5147-2698-3E49-A7CB-548C0D5D350A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F341BDEF-A6D8-D84C-B550-80FC913330B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37800" yWindow="-1980" windowWidth="27240" windowHeight="16260" xr2:uid="{4D476646-5361-4E43-ACF1-036E5CDB58BE}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17260" xr2:uid="{4D476646-5361-4E43-ACF1-036E5CDB58BE}"/>
   </bookViews>
   <sheets>
     <sheet name="WarmF4sept" sheetId="1" r:id="rId1"/>
@@ -942,7 +942,7 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1351,7 +1351,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="C10">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1395,7 +1395,7 @@
         <v>0.375</v>
       </c>
       <c r="C11">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1439,7 +1439,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="C12">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1483,7 +1483,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="C13">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1527,7 +1527,7 @@
         <v>0.5</v>
       </c>
       <c r="C14">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1571,7 +1571,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C15">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1615,7 +1615,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C16">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1659,7 +1659,7 @@
         <v>0.625</v>
       </c>
       <c r="C17">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1703,7 +1703,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C18">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -1747,7 +1747,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="C19">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D19">
         <v>0</v>

</xml_diff>